<commit_message>
Git Actions 연결 세팅
</commit_message>
<xml_diff>
--- a/data/success.xlsx
+++ b/data/success.xlsx
@@ -1611,12 +1611,12 @@
       </c>
       <c r="E2" s="6" t="inlineStr">
         <is>
-          <t>엑셀업로드_0911_1003</t>
+          <t>엑셀업로드_0912_10</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>upload_product_0911_1003</t>
+          <t>upload_product_0912_10</t>
         </is>
       </c>
       <c r="G2" s="3" t="inlineStr">
@@ -1677,12 +1677,12 @@
       </c>
       <c r="E3" s="6" t="inlineStr">
         <is>
-          <t>엑셀업로드_0911_1004</t>
+          <t>엑셀업로드_0912_11</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>upload_product_0911_1004</t>
+          <t>upload_product_0912_11</t>
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr">
@@ -1743,12 +1743,12 @@
       </c>
       <c r="E4" s="6" t="inlineStr">
         <is>
-          <t>엑셀업로드_0911_1005</t>
+          <t>엑셀업로드_0912_12</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>upload_product_0911_1005</t>
+          <t>upload_product_0912_12</t>
         </is>
       </c>
       <c r="G4" s="3" t="inlineStr">

</xml_diff>